<commit_message>
add elsevier apc price data
</commit_message>
<xml_diff>
--- a/ingest/apc/files/elsevier_publishing_charge.xlsx
+++ b/ingest/apc/files/elsevier_publishing_charge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casey/PycharmProjects/journalsdb/ingest/apc/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4BDC60-0691-8341-B044-5704AE6456A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1EECF5-B512-3146-961B-1D553D0D1111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="24160" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8842" uniqueCount="5369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8835" uniqueCount="5380">
   <si>
     <t>Article Publishing Charge (APC) price list</t>
   </si>
@@ -16168,6 +16168,39 @@
   </si>
   <si>
     <t>This journal is a peer reviewed, subsidized open access journal where Beijing University of Chinese Medicine pays for the publishing costs incurred by the journal.</t>
+  </si>
+  <si>
+    <t>However, the Article Publishing Charge (APC) fee will be covered by the "Sociedad Española de Neurología".</t>
+  </si>
+  <si>
+    <t>This journal is a peer reviewed, subsidized open access journal where the Korean Nuclear Society pays for the publishing costs incurred by the journal.</t>
+  </si>
+  <si>
+    <t>This journal is a peer reviewed, subsidized open access journal where The Korean Society of Osteoporosis pays the OA fee.</t>
+  </si>
+  <si>
+    <t>This journal is a peer reviewed, open access journal where Pediatric Hematology Oncology Chapter of Indian Academy of Pediatrics pays the OA fee.</t>
+  </si>
+  <si>
+    <t>This journal is a peer reviewed, subsidized open access journal where the Taiwan Pediatric Association ("the Association") pays for the publishing costs incurred by the journal.</t>
+  </si>
+  <si>
+    <t>This journal is a peer reviewed, subsidized open access journal where the Brazilian Association for Ecological Science and Conservation (ABECO) pays for the publishing costs incurred by the journal.</t>
+  </si>
+  <si>
+    <t>Being discontinued</t>
+  </si>
+  <si>
+    <t>This journal is a peer reviewed, subsidized open access journal where the Chinese Materials Research Society pays the OA fee.</t>
+  </si>
+  <si>
+    <t>This journal is a peer reviewed, subsidized open access journal where the Asian Pacific Prostate Society pays for the publishing costs incurred by the journal.</t>
+  </si>
+  <si>
+    <t>This journal is a peer reviewed, subsidized open access journal where the Sociedade Portuguesa de Pneumologia pays for the publishing costs incurred by the journal.</t>
+  </si>
+  <si>
+    <t>This journal is a peer reviewed, subsidized open access journal where the Sociedade Portuguesa de Cardiologia pays for the publishing costs incurred by the journal.</t>
   </si>
 </sst>
 </file>
@@ -16357,11 +16390,11 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -16757,8 +16790,8 @@
   <dimension ref="A1:H2657"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A1562" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1580" sqref="K1580"/>
+      <pane ySplit="4" topLeftCell="A2233" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2249" sqref="J2249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16770,26 +16803,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
@@ -54828,7 +54861,7 @@
         <v>282640</v>
       </c>
     </row>
-    <row r="1649" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1649" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1649" s="3" t="s">
         <v>3301</v>
       </c>
@@ -54851,7 +54884,7 @@
         <v>343890</v>
       </c>
     </row>
-    <row r="1650" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1650" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1650" s="5" t="s">
         <v>3303</v>
       </c>
@@ -54874,7 +54907,7 @@
         <v>257920</v>
       </c>
     </row>
-    <row r="1651" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1651" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1651" s="3" t="s">
         <v>3305</v>
       </c>
@@ -54897,7 +54930,7 @@
         <v>186990</v>
       </c>
     </row>
-    <row r="1652" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1652" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1652" s="5" t="s">
         <v>3307</v>
       </c>
@@ -54920,7 +54953,7 @@
         <v>306280</v>
       </c>
     </row>
-    <row r="1653" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1653" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1653" s="3" t="s">
         <v>3309</v>
       </c>
@@ -54940,8 +54973,11 @@
       <c r="G1653" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1654" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1653" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1654" s="5" t="s">
         <v>3311</v>
       </c>
@@ -54961,8 +54997,11 @@
       <c r="G1654" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1655" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1654" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1655" s="3" t="s">
         <v>3313</v>
       </c>
@@ -54985,7 +55024,7 @@
         <v>242880</v>
       </c>
     </row>
-    <row r="1656" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1656" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1656" s="5" t="s">
         <v>3315</v>
       </c>
@@ -55008,7 +55047,7 @@
         <v>186990</v>
       </c>
     </row>
-    <row r="1657" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1657" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1657" s="3" t="s">
         <v>3317</v>
       </c>
@@ -55031,7 +55070,7 @@
         <v>295530</v>
       </c>
     </row>
-    <row r="1658" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1658" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1658" s="5" t="s">
         <v>3319</v>
       </c>
@@ -55054,7 +55093,7 @@
         <v>85970</v>
       </c>
     </row>
-    <row r="1659" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1659" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1659" s="3" t="s">
         <v>3321</v>
       </c>
@@ -55077,7 +55116,7 @@
         <v>187870</v>
       </c>
     </row>
-    <row r="1660" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1660" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1660" s="5" t="s">
         <v>3323</v>
       </c>
@@ -55100,7 +55139,7 @@
         <v>207410</v>
       </c>
     </row>
-    <row r="1661" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1661" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1661" s="3" t="s">
         <v>3325</v>
       </c>
@@ -55120,8 +55159,11 @@
       <c r="G1661" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1662" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1661" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1662" s="5" t="s">
         <v>3327</v>
       </c>
@@ -55141,8 +55183,11 @@
       <c r="G1662" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1663" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1662" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1663" s="3" t="s">
         <v>3329</v>
       </c>
@@ -55165,7 +55210,7 @@
         <v>186990</v>
       </c>
     </row>
-    <row r="1664" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1664" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1664" s="5" t="s">
         <v>3331</v>
       </c>
@@ -55185,6 +55230,9 @@
       <c r="G1664" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="H1664" s="11" t="s">
+        <v>5342</v>
+      </c>
     </row>
     <row r="1665" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1665" s="3" t="s">
@@ -55840,8 +55888,8 @@
       <c r="C1693" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1693" s="7" t="s">
-        <v>42</v>
+      <c r="D1693" s="7">
+        <v>2200</v>
       </c>
       <c r="E1693" s="7" t="s">
         <v>42</v>
@@ -57026,7 +57074,7 @@
         <v>328850</v>
       </c>
     </row>
-    <row r="1745" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1745" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1745" s="3" t="s">
         <v>3493</v>
       </c>
@@ -57049,7 +57097,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1746" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1746" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1746" s="5" t="s">
         <v>3495</v>
       </c>
@@ -57072,7 +57120,7 @@
         <v>354640</v>
       </c>
     </row>
-    <row r="1747" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1747" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1747" s="3" t="s">
         <v>3497</v>
       </c>
@@ -57095,7 +57143,7 @@
         <v>295530</v>
       </c>
     </row>
-    <row r="1748" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1748" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1748" s="5" t="s">
         <v>3499</v>
       </c>
@@ -57118,7 +57166,7 @@
         <v>229980</v>
       </c>
     </row>
-    <row r="1749" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1749" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1749" s="3" t="s">
         <v>3501</v>
       </c>
@@ -57141,7 +57189,7 @@
         <v>956500</v>
       </c>
     </row>
-    <row r="1750" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1750" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1750" s="5" t="s">
         <v>3503</v>
       </c>
@@ -57164,7 +57212,7 @@
         <v>360010</v>
       </c>
     </row>
-    <row r="1751" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1751" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1751" s="3" t="s">
         <v>3505</v>
       </c>
@@ -57187,7 +57235,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="1752" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1752" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1752" s="5" t="s">
         <v>3507</v>
       </c>
@@ -57210,7 +57258,7 @@
         <v>309500</v>
       </c>
     </row>
-    <row r="1753" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1753" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1753" s="3" t="s">
         <v>3509</v>
       </c>
@@ -57233,7 +57281,7 @@
         <v>198810</v>
       </c>
     </row>
-    <row r="1754" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1754" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1754" s="5" t="s">
         <v>3511</v>
       </c>
@@ -57256,7 +57304,7 @@
         <v>426640</v>
       </c>
     </row>
-    <row r="1755" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1755" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1755" s="3" t="s">
         <v>3513</v>
       </c>
@@ -57276,8 +57324,11 @@
       <c r="G1755" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1756" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1755" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1756" s="5" t="s">
         <v>3515</v>
       </c>
@@ -57300,7 +57351,7 @@
         <v>48360</v>
       </c>
     </row>
-    <row r="1757" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1757" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1757" s="3" t="s">
         <v>3517</v>
       </c>
@@ -57323,7 +57374,7 @@
         <v>300910</v>
       </c>
     </row>
-    <row r="1758" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1758" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1758" s="5" t="s">
         <v>3519</v>
       </c>
@@ -57346,7 +57397,7 @@
         <v>217080</v>
       </c>
     </row>
-    <row r="1759" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1759" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1759" s="3" t="s">
         <v>3521</v>
       </c>
@@ -57369,7 +57420,7 @@
         <v>186990</v>
       </c>
     </row>
-    <row r="1760" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1760" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1760" s="5" t="s">
         <v>3523</v>
       </c>
@@ -57390,7 +57441,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="1761" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1761" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1761" s="3" t="s">
         <v>3525</v>
       </c>
@@ -57413,7 +57464,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1762" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1762" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1762" s="5" t="s">
         <v>3527</v>
       </c>
@@ -57436,7 +57487,7 @@
         <v>186990</v>
       </c>
     </row>
-    <row r="1763" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1763" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1763" s="3" t="s">
         <v>3529</v>
       </c>
@@ -57459,7 +57510,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="1764" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1764" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1764" s="5" t="s">
         <v>3531</v>
       </c>
@@ -57482,7 +57533,7 @@
         <v>294460</v>
       </c>
     </row>
-    <row r="1765" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="1765" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A1765" s="3" t="s">
         <v>3533</v>
       </c>
@@ -57502,8 +57553,11 @@
       <c r="G1765" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1766" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1765" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1766" s="5" t="s">
         <v>3535</v>
       </c>
@@ -57526,7 +57580,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1767" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1767" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1767" s="3" t="s">
         <v>3537</v>
       </c>
@@ -57549,7 +57603,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1768" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1768" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1768" s="5" t="s">
         <v>3539</v>
       </c>
@@ -57572,7 +57626,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1769" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1769" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1769" s="3" t="s">
         <v>3541</v>
       </c>
@@ -57595,7 +57649,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1770" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1770" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1770" s="5" t="s">
         <v>3543</v>
       </c>
@@ -57615,8 +57669,11 @@
       <c r="G1770" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1771" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1770" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1771" s="3" t="s">
         <v>3545</v>
       </c>
@@ -57639,7 +57696,7 @@
         <v>257920</v>
       </c>
     </row>
-    <row r="1772" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1772" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1772" s="5" t="s">
         <v>3547</v>
       </c>
@@ -57662,7 +57719,7 @@
         <v>249320</v>
       </c>
     </row>
-    <row r="1773" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1773" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1773" s="3" t="s">
         <v>3549</v>
       </c>
@@ -57685,7 +57742,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="1774" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1774" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1774" s="5" t="s">
         <v>3551</v>
       </c>
@@ -57708,7 +57765,7 @@
         <v>475000</v>
       </c>
     </row>
-    <row r="1775" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1775" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1775" s="3" t="s">
         <v>3553</v>
       </c>
@@ -57731,7 +57788,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="1776" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1776" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1776" s="5" t="s">
         <v>3555</v>
       </c>
@@ -58858,7 +58915,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1825" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1825" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1825" s="3" t="s">
         <v>3653</v>
       </c>
@@ -58881,7 +58938,7 @@
         <v>237500</v>
       </c>
     </row>
-    <row r="1826" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1826" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1826" s="5" t="s">
         <v>3655</v>
       </c>
@@ -58904,7 +58961,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1827" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1827" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1827" s="3" t="s">
         <v>3657</v>
       </c>
@@ -58927,7 +58984,7 @@
         <v>161200</v>
       </c>
     </row>
-    <row r="1828" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1828" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1828" s="5" t="s">
         <v>3659</v>
       </c>
@@ -58950,7 +59007,7 @@
         <v>249320</v>
       </c>
     </row>
-    <row r="1829" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1829" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1829" s="3" t="s">
         <v>3661</v>
       </c>
@@ -58970,8 +59027,11 @@
       <c r="G1829" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1830" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1829" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1830" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1830" s="5" t="s">
         <v>3663</v>
       </c>
@@ -58994,7 +59054,7 @@
         <v>212780</v>
       </c>
     </row>
-    <row r="1831" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1831" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1831" s="3" t="s">
         <v>3665</v>
       </c>
@@ -59017,7 +59077,7 @@
         <v>424490</v>
       </c>
     </row>
-    <row r="1832" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1832" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1832" s="5" t="s">
         <v>3667</v>
       </c>
@@ -59040,7 +59100,7 @@
         <v>425570</v>
       </c>
     </row>
-    <row r="1833" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1833" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1833" s="3" t="s">
         <v>3669</v>
       </c>
@@ -59063,7 +59123,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1834" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1834" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1834" s="5" t="s">
         <v>3671</v>
       </c>
@@ -59086,7 +59146,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1835" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1835" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1835" s="3" t="s">
         <v>3673</v>
       </c>
@@ -59109,7 +59169,7 @@
         <v>346040</v>
       </c>
     </row>
-    <row r="1836" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1836" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1836" s="5" t="s">
         <v>3675</v>
       </c>
@@ -59132,7 +59192,7 @@
         <v>380430</v>
       </c>
     </row>
-    <row r="1837" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1837" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1837" s="3" t="s">
         <v>3677</v>
       </c>
@@ -59142,20 +59202,23 @@
       <c r="C1837" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1837" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1837" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1837" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1837" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="1838" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D1837" s="7">
+        <v>0</v>
+      </c>
+      <c r="E1837" s="7">
+        <v>0</v>
+      </c>
+      <c r="F1837" s="7">
+        <v>0</v>
+      </c>
+      <c r="G1837" s="7">
+        <v>0</v>
+      </c>
+      <c r="H1837" t="s">
+        <v>5323</v>
+      </c>
+    </row>
+    <row r="1838" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1838" s="5" t="s">
         <v>3679</v>
       </c>
@@ -59165,20 +59228,23 @@
       <c r="C1838" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1838" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1838" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1838" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1838" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="1839" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D1838" s="8">
+        <v>0</v>
+      </c>
+      <c r="E1838" s="8">
+        <v>0</v>
+      </c>
+      <c r="F1838" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1838" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1838" t="s">
+        <v>5323</v>
+      </c>
+    </row>
+    <row r="1839" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1839" s="3" t="s">
         <v>3681</v>
       </c>
@@ -59201,7 +59267,7 @@
         <v>300910</v>
       </c>
     </row>
-    <row r="1840" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1840" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1840" s="5" t="s">
         <v>3683</v>
       </c>
@@ -59224,7 +59290,7 @@
         <v>150450</v>
       </c>
     </row>
-    <row r="1841" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1841" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1841" s="3" t="s">
         <v>3685</v>
       </c>
@@ -59247,7 +59313,7 @@
         <v>360010</v>
       </c>
     </row>
-    <row r="1842" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1842" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1842" s="5" t="s">
         <v>3687</v>
       </c>
@@ -59270,7 +59336,7 @@
         <v>343890</v>
       </c>
     </row>
-    <row r="1843" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1843" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1843" s="3" t="s">
         <v>3689</v>
       </c>
@@ -59293,7 +59359,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1844" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1844" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1844" s="5" t="s">
         <v>3691</v>
       </c>
@@ -59316,7 +59382,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="1845" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1845" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1845" s="3" t="s">
         <v>3693</v>
       </c>
@@ -59339,7 +59405,7 @@
         <v>338520</v>
       </c>
     </row>
-    <row r="1846" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1846" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1846" s="5" t="s">
         <v>3695</v>
       </c>
@@ -59362,7 +59428,7 @@
         <v>177320</v>
       </c>
     </row>
-    <row r="1847" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1847" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1847" s="3" t="s">
         <v>3697</v>
       </c>
@@ -59385,7 +59451,7 @@
         <v>212780</v>
       </c>
     </row>
-    <row r="1848" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1848" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1848" s="5" t="s">
         <v>3699</v>
       </c>
@@ -59408,7 +59474,7 @@
         <v>353570</v>
       </c>
     </row>
-    <row r="1849" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1849" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1849" s="3" t="s">
         <v>3701</v>
       </c>
@@ -59431,7 +59497,7 @@
         <v>317030</v>
       </c>
     </row>
-    <row r="1850" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1850" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1850" s="5" t="s">
         <v>3703</v>
       </c>
@@ -59454,7 +59520,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1851" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1851" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1851" s="3" t="s">
         <v>3705</v>
       </c>
@@ -59475,7 +59541,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="1852" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1852" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1852" s="5" t="s">
         <v>3707</v>
       </c>
@@ -59483,8 +59549,8 @@
         <v>3708</v>
       </c>
       <c r="C1852" s="5"/>
-      <c r="D1852" s="8" t="s">
-        <v>42</v>
+      <c r="D1852" s="8">
+        <v>2500</v>
       </c>
       <c r="E1852" s="8" t="s">
         <v>42</v>
@@ -59496,7 +59562,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="1853" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1853" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1853" s="3" t="s">
         <v>3709</v>
       </c>
@@ -59519,7 +59585,7 @@
         <v>257920</v>
       </c>
     </row>
-    <row r="1854" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1854" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1854" s="5" t="s">
         <v>3711</v>
       </c>
@@ -59542,7 +59608,7 @@
         <v>354640</v>
       </c>
     </row>
-    <row r="1855" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1855" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1855" s="3" t="s">
         <v>3713</v>
       </c>
@@ -59565,7 +59631,7 @@
         <v>338520</v>
       </c>
     </row>
-    <row r="1856" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1856" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1856" s="5" t="s">
         <v>3715</v>
       </c>
@@ -59575,20 +59641,23 @@
       <c r="C1856" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1856" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1856" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1856" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1856" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="1857" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D1856" s="8">
+        <v>0</v>
+      </c>
+      <c r="E1856" s="8">
+        <v>0</v>
+      </c>
+      <c r="F1856" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1856" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1856" t="s">
+        <v>5351</v>
+      </c>
+    </row>
+    <row r="1857" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1857" s="3" t="s">
         <v>3717</v>
       </c>
@@ -59611,7 +59680,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1858" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1858" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1858" s="5" t="s">
         <v>3719</v>
       </c>
@@ -59634,7 +59703,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1859" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1859" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1859" s="3" t="s">
         <v>3721</v>
       </c>
@@ -59657,7 +59726,7 @@
         <v>392250</v>
       </c>
     </row>
-    <row r="1860" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1860" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1860" s="5" t="s">
         <v>3723</v>
       </c>
@@ -59680,7 +59749,7 @@
         <v>159560</v>
       </c>
     </row>
-    <row r="1861" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1861" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1861" s="3" t="s">
         <v>3725</v>
       </c>
@@ -59703,7 +59772,7 @@
         <v>224610</v>
       </c>
     </row>
-    <row r="1862" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1862" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1862" s="5" t="s">
         <v>3727</v>
       </c>
@@ -59713,20 +59782,23 @@
       <c r="C1862" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1862" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1862" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1862" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1862" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="1863" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D1862" s="8">
+        <v>0</v>
+      </c>
+      <c r="E1862" s="8">
+        <v>0</v>
+      </c>
+      <c r="F1862" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1862" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1862" t="s">
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1863" s="3" t="s">
         <v>3729</v>
       </c>
@@ -59746,8 +59818,11 @@
       <c r="G1863" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1864" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1863" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1864" s="5" t="s">
         <v>3731</v>
       </c>
@@ -59770,7 +59845,7 @@
         <v>333150</v>
       </c>
     </row>
-    <row r="1865" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1865" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1865" s="3" t="s">
         <v>3733</v>
       </c>
@@ -59793,7 +59868,7 @@
         <v>956500</v>
       </c>
     </row>
-    <row r="1866" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1866" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1866" s="5" t="s">
         <v>3735</v>
       </c>
@@ -59816,7 +59891,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1867" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1867" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1867" s="3" t="s">
         <v>3737</v>
       </c>
@@ -59839,7 +59914,7 @@
         <v>381510</v>
       </c>
     </row>
-    <row r="1868" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1868" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1868" s="5" t="s">
         <v>3739</v>
       </c>
@@ -59862,7 +59937,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1869" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1869" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1869" s="3" t="s">
         <v>3741</v>
       </c>
@@ -59885,7 +59960,7 @@
         <v>186990</v>
       </c>
     </row>
-    <row r="1870" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1870" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1870" s="5" t="s">
         <v>3743</v>
       </c>
@@ -59908,7 +59983,7 @@
         <v>306280</v>
       </c>
     </row>
-    <row r="1871" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1871" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1871" s="3" t="s">
         <v>3745</v>
       </c>
@@ -59931,7 +60006,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1872" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1872" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1872" s="5" t="s">
         <v>3747</v>
       </c>
@@ -59954,7 +60029,7 @@
         <v>466410</v>
       </c>
     </row>
-    <row r="1873" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1873" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1873" s="3" t="s">
         <v>3749</v>
       </c>
@@ -59977,7 +60052,7 @@
         <v>297680</v>
       </c>
     </row>
-    <row r="1874" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1874" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1874" s="5" t="s">
         <v>3751</v>
       </c>
@@ -60000,7 +60075,7 @@
         <v>263290</v>
       </c>
     </row>
-    <row r="1875" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1875" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1875" s="3" t="s">
         <v>3753</v>
       </c>
@@ -60023,7 +60098,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1876" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1876" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1876" s="5" t="s">
         <v>3755</v>
       </c>
@@ -60046,7 +60121,7 @@
         <v>362160</v>
       </c>
     </row>
-    <row r="1877" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1877" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1877" s="3" t="s">
         <v>3757</v>
       </c>
@@ -60069,7 +60144,7 @@
         <v>343890</v>
       </c>
     </row>
-    <row r="1878" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1878" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1878" s="5" t="s">
         <v>3759</v>
       </c>
@@ -60092,7 +60167,7 @@
         <v>212780</v>
       </c>
     </row>
-    <row r="1879" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1879" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1879" s="3" t="s">
         <v>3761</v>
       </c>
@@ -60115,7 +60190,7 @@
         <v>236430</v>
       </c>
     </row>
-    <row r="1880" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1880" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1880" s="5" t="s">
         <v>3763</v>
       </c>
@@ -60138,7 +60213,7 @@
         <v>376130</v>
       </c>
     </row>
-    <row r="1881" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1881" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1881" s="3" t="s">
         <v>3765</v>
       </c>
@@ -60158,8 +60233,11 @@
       <c r="G1881" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1882" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1881" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1882" s="5" t="s">
         <v>3767</v>
       </c>
@@ -60182,7 +60260,7 @@
         <v>332070</v>
       </c>
     </row>
-    <row r="1883" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1883" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1883" s="3" t="s">
         <v>3769</v>
       </c>
@@ -60205,7 +60283,7 @@
         <v>195590</v>
       </c>
     </row>
-    <row r="1884" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1884" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1884" s="5" t="s">
         <v>3771</v>
       </c>
@@ -60228,7 +60306,7 @@
         <v>150450</v>
       </c>
     </row>
-    <row r="1885" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1885" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1885" s="3" t="s">
         <v>3773</v>
       </c>
@@ -60251,7 +60329,7 @@
         <v>134330</v>
       </c>
     </row>
-    <row r="1886" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1886" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1886" s="5" t="s">
         <v>3775</v>
       </c>
@@ -60274,7 +60352,7 @@
         <v>263290</v>
       </c>
     </row>
-    <row r="1887" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1887" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1887" s="3" t="s">
         <v>3777</v>
       </c>
@@ -60297,7 +60375,7 @@
         <v>247170</v>
       </c>
     </row>
-    <row r="1888" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1888" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1888" s="5" t="s">
         <v>3779</v>
       </c>
@@ -60320,7 +60398,7 @@
         <v>289090</v>
       </c>
     </row>
-    <row r="1889" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1889" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1889" s="3" t="s">
         <v>3781</v>
       </c>
@@ -60343,7 +60421,7 @@
         <v>306280</v>
       </c>
     </row>
-    <row r="1890" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1890" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1890" s="5" t="s">
         <v>3783</v>
       </c>
@@ -60366,7 +60444,7 @@
         <v>220310</v>
       </c>
     </row>
-    <row r="1891" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1891" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1891" s="3" t="s">
         <v>3785</v>
       </c>
@@ -60389,7 +60467,7 @@
         <v>225680</v>
       </c>
     </row>
-    <row r="1892" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1892" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1892" s="5" t="s">
         <v>3787</v>
       </c>
@@ -60412,7 +60490,7 @@
         <v>266520</v>
       </c>
     </row>
-    <row r="1893" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1893" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1893" s="3" t="s">
         <v>3789</v>
       </c>
@@ -60435,7 +60513,7 @@
         <v>290160</v>
       </c>
     </row>
-    <row r="1894" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1894" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1894" s="5" t="s">
         <v>3791</v>
       </c>
@@ -60458,7 +60536,7 @@
         <v>343890</v>
       </c>
     </row>
-    <row r="1895" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1895" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1895" s="3" t="s">
         <v>3793</v>
       </c>
@@ -60481,7 +60559,7 @@
         <v>250400</v>
       </c>
     </row>
-    <row r="1896" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1896" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1896" s="5" t="s">
         <v>3795</v>
       </c>
@@ -60491,20 +60569,23 @@
       <c r="C1896" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1896" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1896" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1896" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1896" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="1897" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="D1896" s="8">
+        <v>0</v>
+      </c>
+      <c r="E1896" s="8">
+        <v>0</v>
+      </c>
+      <c r="F1896" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1896" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1896" t="s">
+        <v>5370</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A1897" s="3" t="s">
         <v>3797</v>
       </c>
@@ -60527,7 +60608,7 @@
         <v>289090</v>
       </c>
     </row>
-    <row r="1898" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="1898" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A1898" s="5" t="s">
         <v>3799</v>
       </c>
@@ -60550,7 +60631,7 @@
         <v>274040</v>
       </c>
     </row>
-    <row r="1899" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1899" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1899" s="3" t="s">
         <v>3801</v>
       </c>
@@ -60573,7 +60654,7 @@
         <v>118210</v>
       </c>
     </row>
-    <row r="1900" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1900" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1900" s="5" t="s">
         <v>3803</v>
       </c>
@@ -60596,7 +60677,7 @@
         <v>351420</v>
       </c>
     </row>
-    <row r="1901" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1901" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1901" s="3" t="s">
         <v>3805</v>
       </c>
@@ -60619,7 +60700,7 @@
         <v>209560</v>
       </c>
     </row>
-    <row r="1902" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1902" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1902" s="5" t="s">
         <v>3807</v>
       </c>
@@ -60641,8 +60722,11 @@
       <c r="G1902" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1903" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1902" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1903" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1903" s="3" t="s">
         <v>3809</v>
       </c>
@@ -60665,7 +60749,7 @@
         <v>290160</v>
       </c>
     </row>
-    <row r="1904" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1904" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1904" s="5" t="s">
         <v>3811</v>
       </c>
@@ -60688,7 +60772,7 @@
         <v>406230</v>
       </c>
     </row>
-    <row r="1905" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1905" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1905" s="3" t="s">
         <v>3813</v>
       </c>
@@ -60711,7 +60795,7 @@
         <v>263290</v>
       </c>
     </row>
-    <row r="1906" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1906" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1906" s="5" t="s">
         <v>3815</v>
       </c>
@@ -60734,7 +60818,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1907" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1907" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1907" s="3" t="s">
         <v>3817</v>
       </c>
@@ -60757,7 +60841,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1908" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1908" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1908" s="5" t="s">
         <v>3819</v>
       </c>
@@ -60780,7 +60864,7 @@
         <v>295530</v>
       </c>
     </row>
-    <row r="1909" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1909" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1909" s="3" t="s">
         <v>3821</v>
       </c>
@@ -60803,7 +60887,7 @@
         <v>306280</v>
       </c>
     </row>
-    <row r="1910" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1910" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1910" s="5" t="s">
         <v>3823</v>
       </c>
@@ -60826,7 +60910,7 @@
         <v>124660</v>
       </c>
     </row>
-    <row r="1911" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1911" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1911" s="3" t="s">
         <v>3825</v>
       </c>
@@ -60849,7 +60933,7 @@
         <v>327770</v>
       </c>
     </row>
-    <row r="1912" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1912" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1912" s="5" t="s">
         <v>3827</v>
       </c>
@@ -60872,7 +60956,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1913" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1913" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1913" s="3" t="s">
         <v>3829</v>
       </c>
@@ -60895,7 +60979,7 @@
         <v>247170</v>
       </c>
     </row>
-    <row r="1914" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1914" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1914" s="5" t="s">
         <v>3831</v>
       </c>
@@ -60918,7 +61002,7 @@
         <v>300910</v>
       </c>
     </row>
-    <row r="1915" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1915" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1915" s="3" t="s">
         <v>3833</v>
       </c>
@@ -60941,7 +61025,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1916" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1916" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1916" s="5" t="s">
         <v>3835</v>
       </c>
@@ -60964,7 +61048,7 @@
         <v>300910</v>
       </c>
     </row>
-    <row r="1917" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1917" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1917" s="3" t="s">
         <v>3837</v>
       </c>
@@ -60987,7 +61071,7 @@
         <v>343890</v>
       </c>
     </row>
-    <row r="1918" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1918" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1918" s="5" t="s">
         <v>3839</v>
       </c>
@@ -61010,7 +61094,7 @@
         <v>346040</v>
       </c>
     </row>
-    <row r="1919" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1919" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1919" s="3" t="s">
         <v>3841</v>
       </c>
@@ -61033,7 +61117,7 @@
         <v>353570</v>
       </c>
     </row>
-    <row r="1920" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1920" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1920" s="5" t="s">
         <v>3843</v>
       </c>
@@ -61054,6 +61138,9 @@
       </c>
       <c r="G1920" s="8" t="s">
         <v>42</v>
+      </c>
+      <c r="H1920" s="11" t="s">
+        <v>5342</v>
       </c>
     </row>
     <row r="1921" spans="1:7" x14ac:dyDescent="0.2">
@@ -61790,7 +61877,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="1953" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1953" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1953" s="3" t="s">
         <v>3909</v>
       </c>
@@ -61813,7 +61900,7 @@
         <v>335300</v>
       </c>
     </row>
-    <row r="1954" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1954" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1954" s="5" t="s">
         <v>3911</v>
       </c>
@@ -61836,7 +61923,7 @@
         <v>284790</v>
       </c>
     </row>
-    <row r="1955" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1955" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1955" s="3" t="s">
         <v>3913</v>
       </c>
@@ -61859,7 +61946,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="1956" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1956" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1956" s="5" t="s">
         <v>3915</v>
       </c>
@@ -61882,7 +61969,7 @@
         <v>254700</v>
       </c>
     </row>
-    <row r="1957" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1957" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1957" s="3" t="s">
         <v>3917</v>
       </c>
@@ -61905,7 +61992,7 @@
         <v>307360</v>
       </c>
     </row>
-    <row r="1958" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1958" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1958" s="5" t="s">
         <v>3919</v>
       </c>
@@ -61928,7 +62015,7 @@
         <v>204190</v>
       </c>
     </row>
-    <row r="1959" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1959" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1959" s="3" t="s">
         <v>3921</v>
       </c>
@@ -61951,7 +62038,7 @@
         <v>338520</v>
       </c>
     </row>
-    <row r="1960" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1960" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1960" s="5" t="s">
         <v>3923</v>
       </c>
@@ -61974,7 +62061,7 @@
         <v>263290</v>
       </c>
     </row>
-    <row r="1961" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1961" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1961" s="3" t="s">
         <v>3925</v>
       </c>
@@ -61997,7 +62084,7 @@
         <v>424490</v>
       </c>
     </row>
-    <row r="1962" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1962" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1962" s="5" t="s">
         <v>3927</v>
       </c>
@@ -62020,7 +62107,7 @@
         <v>182690</v>
       </c>
     </row>
-    <row r="1963" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1963" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1963" s="3" t="s">
         <v>3929</v>
       </c>
@@ -62043,7 +62130,7 @@
         <v>278340</v>
       </c>
     </row>
-    <row r="1964" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1964" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1964" s="5" t="s">
         <v>3931</v>
       </c>
@@ -62066,7 +62153,7 @@
         <v>150450</v>
       </c>
     </row>
-    <row r="1965" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1965" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1965" s="3" t="s">
         <v>3933</v>
       </c>
@@ -62089,7 +62176,7 @@
         <v>254700</v>
       </c>
     </row>
-    <row r="1966" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1966" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1966" s="5" t="s">
         <v>3935</v>
       </c>
@@ -62099,20 +62186,23 @@
       <c r="C1966" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1966" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1966" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1966" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1966" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="1967" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D1966" s="8">
+        <v>0</v>
+      </c>
+      <c r="E1966" s="8">
+        <v>0</v>
+      </c>
+      <c r="F1966" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1966" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1966" t="s">
+        <v>5371</v>
+      </c>
+    </row>
+    <row r="1967" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1967" s="3" t="s">
         <v>3937</v>
       </c>
@@ -62135,7 +62225,7 @@
         <v>348190</v>
       </c>
     </row>
-    <row r="1968" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1968" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1968" s="5" t="s">
         <v>3939</v>
       </c>
@@ -62158,7 +62248,7 @@
         <v>80600</v>
       </c>
     </row>
-    <row r="1969" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1969" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1969" s="3" t="s">
         <v>3941</v>
       </c>
@@ -62178,8 +62268,11 @@
       <c r="G1969" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1970" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1969" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1970" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1970" s="5" t="s">
         <v>3943</v>
       </c>
@@ -62202,7 +62295,7 @@
         <v>212780</v>
       </c>
     </row>
-    <row r="1971" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1971" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1971" s="3" t="s">
         <v>3945</v>
       </c>
@@ -62225,7 +62318,7 @@
         <v>356790</v>
       </c>
     </row>
-    <row r="1972" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1972" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1972" s="5" t="s">
         <v>3947</v>
       </c>
@@ -62248,7 +62341,7 @@
         <v>279410</v>
       </c>
     </row>
-    <row r="1973" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1973" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1973" s="3" t="s">
         <v>3949</v>
       </c>
@@ -62271,7 +62364,7 @@
         <v>303060</v>
       </c>
     </row>
-    <row r="1974" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1974" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1974" s="5" t="s">
         <v>3951</v>
       </c>
@@ -62294,7 +62387,7 @@
         <v>311650</v>
       </c>
     </row>
-    <row r="1975" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1975" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1975" s="3" t="s">
         <v>3953</v>
       </c>
@@ -62317,7 +62410,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1976" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1976" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1976" s="5" t="s">
         <v>3955</v>
       </c>
@@ -62340,7 +62433,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1977" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1977" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1977" s="3" t="s">
         <v>3957</v>
       </c>
@@ -62363,7 +62456,7 @@
         <v>279410</v>
       </c>
     </row>
-    <row r="1978" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1978" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1978" s="5" t="s">
         <v>3959</v>
       </c>
@@ -62386,7 +62479,7 @@
         <v>193440</v>
       </c>
     </row>
-    <row r="1979" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1979" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1979" s="3" t="s">
         <v>3961</v>
       </c>
@@ -62409,7 +62502,7 @@
         <v>295530</v>
       </c>
     </row>
-    <row r="1980" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1980" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1980" s="5" t="s">
         <v>3963</v>
       </c>
@@ -62432,7 +62525,7 @@
         <v>364310</v>
       </c>
     </row>
-    <row r="1981" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1981" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1981" s="3" t="s">
         <v>3965</v>
       </c>
@@ -62442,8 +62535,8 @@
       <c r="C1981" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1981" s="7" t="s">
-        <v>42</v>
+      <c r="D1981" s="7">
+        <v>1000</v>
       </c>
       <c r="E1981" s="7" t="s">
         <v>42</v>
@@ -62455,7 +62548,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="1982" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1982" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1982" s="5" t="s">
         <v>3967</v>
       </c>
@@ -62478,7 +62571,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1983" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1983" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1983" s="3" t="s">
         <v>3969</v>
       </c>
@@ -62501,7 +62594,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="1984" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1984" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1984" s="5" t="s">
         <v>3971</v>
       </c>
@@ -62524,7 +62617,7 @@
         <v>255770</v>
       </c>
     </row>
-    <row r="1985" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1985" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1985" s="3" t="s">
         <v>3973</v>
       </c>
@@ -62547,7 +62640,7 @@
         <v>360010</v>
       </c>
     </row>
-    <row r="1986" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1986" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1986" s="5" t="s">
         <v>3975</v>
       </c>
@@ -62570,7 +62663,7 @@
         <v>333150</v>
       </c>
     </row>
-    <row r="1987" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1987" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1987" s="3" t="s">
         <v>3977</v>
       </c>
@@ -62593,7 +62686,7 @@
         <v>236430</v>
       </c>
     </row>
-    <row r="1988" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1988" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1988" s="5" t="s">
         <v>3979</v>
       </c>
@@ -62616,7 +62709,7 @@
         <v>956500</v>
       </c>
     </row>
-    <row r="1989" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1989" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1989" s="3" t="s">
         <v>3981</v>
       </c>
@@ -62639,7 +62732,7 @@
         <v>274040</v>
       </c>
     </row>
-    <row r="1990" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1990" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1990" s="5" t="s">
         <v>3983</v>
       </c>
@@ -62649,20 +62742,23 @@
       <c r="C1990" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1990" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1990" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1990" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1990" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="1991" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D1990" s="8">
+        <v>0</v>
+      </c>
+      <c r="E1990" s="8">
+        <v>0</v>
+      </c>
+      <c r="F1990" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1990" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1990" t="s">
+        <v>5372</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1991" s="3" t="s">
         <v>3985</v>
       </c>
@@ -62685,7 +62781,7 @@
         <v>290160</v>
       </c>
     </row>
-    <row r="1992" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1992" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1992" s="5" t="s">
         <v>3987</v>
       </c>
@@ -62695,20 +62791,23 @@
       <c r="C1992" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1992" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1992" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1992" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1992" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="1993" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D1992" s="8">
+        <v>0</v>
+      </c>
+      <c r="E1992" s="8">
+        <v>0</v>
+      </c>
+      <c r="F1992" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1992" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1992" t="s">
+        <v>5373</v>
+      </c>
+    </row>
+    <row r="1993" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1993" s="3" t="s">
         <v>3989</v>
       </c>
@@ -62731,7 +62830,7 @@
         <v>225680</v>
       </c>
     </row>
-    <row r="1994" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1994" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1994" s="5" t="s">
         <v>3991</v>
       </c>
@@ -62751,8 +62850,11 @@
       <c r="G1994" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="1995" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1994" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1995" s="3" t="s">
         <v>3993</v>
       </c>
@@ -62775,7 +62877,7 @@
         <v>290160</v>
       </c>
     </row>
-    <row r="1996" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1996" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1996" s="5" t="s">
         <v>3995</v>
       </c>
@@ -62798,7 +62900,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="1997" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1997" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1997" s="3" t="s">
         <v>3997</v>
       </c>
@@ -62821,7 +62923,7 @@
         <v>249320</v>
       </c>
     </row>
-    <row r="1998" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1998" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1998" s="5" t="s">
         <v>3999</v>
       </c>
@@ -62844,7 +62946,7 @@
         <v>300910</v>
       </c>
     </row>
-    <row r="1999" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1999" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1999" s="3" t="s">
         <v>4001</v>
       </c>
@@ -62867,7 +62969,7 @@
         <v>263290</v>
       </c>
     </row>
-    <row r="2000" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2000" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2000" s="5" t="s">
         <v>4003</v>
       </c>
@@ -62890,7 +62992,7 @@
         <v>306280</v>
       </c>
     </row>
-    <row r="2001" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2001" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2001" s="3" t="s">
         <v>4005</v>
       </c>
@@ -62913,7 +63015,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="2002" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2002" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2002" s="5" t="s">
         <v>4007</v>
       </c>
@@ -62923,20 +63025,23 @@
       <c r="C2002" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2002" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2002" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2002" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2002" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2003" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2002" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2002" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2002" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2002" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2002" t="s">
+        <v>5374</v>
+      </c>
+    </row>
+    <row r="2003" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2003" s="3" t="s">
         <v>4009</v>
       </c>
@@ -62959,7 +63064,7 @@
         <v>306280</v>
       </c>
     </row>
-    <row r="2004" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2004" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2004" s="5" t="s">
         <v>4011</v>
       </c>
@@ -62982,7 +63087,7 @@
         <v>241800</v>
       </c>
     </row>
-    <row r="2005" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2005" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2005" s="3" t="s">
         <v>4013</v>
       </c>
@@ -63005,7 +63110,7 @@
         <v>377210</v>
       </c>
     </row>
-    <row r="2006" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2006" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2006" s="5" t="s">
         <v>4015</v>
       </c>
@@ -63028,7 +63133,7 @@
         <v>365390</v>
       </c>
     </row>
-    <row r="2007" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2007" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2007" s="3" t="s">
         <v>4017</v>
       </c>
@@ -63051,7 +63156,7 @@
         <v>376130</v>
       </c>
     </row>
-    <row r="2008" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2008" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2008" s="5" t="s">
         <v>4019</v>
       </c>
@@ -63074,7 +63179,7 @@
         <v>150450</v>
       </c>
     </row>
-    <row r="2009" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2009" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2009" s="3" t="s">
         <v>4021</v>
       </c>
@@ -63097,7 +63202,7 @@
         <v>475000</v>
       </c>
     </row>
-    <row r="2010" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2010" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2010" s="5" t="s">
         <v>4023</v>
       </c>
@@ -63120,7 +63225,7 @@
         <v>303060</v>
       </c>
     </row>
-    <row r="2011" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2011" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2011" s="3" t="s">
         <v>4025</v>
       </c>
@@ -63140,8 +63245,11 @@
       <c r="G2011" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2012" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2011" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2012" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2012" s="5" t="s">
         <v>4027</v>
       </c>
@@ -63164,7 +63272,7 @@
         <v>293380</v>
       </c>
     </row>
-    <row r="2013" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2013" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2013" s="3" t="s">
         <v>4029</v>
       </c>
@@ -63187,7 +63295,7 @@
         <v>222460</v>
       </c>
     </row>
-    <row r="2014" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2014" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2014" s="5" t="s">
         <v>4031</v>
       </c>
@@ -63210,7 +63318,7 @@
         <v>347120</v>
       </c>
     </row>
-    <row r="2015" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="2015" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2015" s="3" t="s">
         <v>4033</v>
       </c>
@@ -63233,7 +63341,7 @@
         <v>266520</v>
       </c>
     </row>
-    <row r="2016" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2016" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2016" s="5" t="s">
         <v>4035</v>
       </c>
@@ -63256,7 +63364,7 @@
         <v>245020</v>
       </c>
     </row>
-    <row r="2017" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2017" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2017" s="3" t="s">
         <v>4037</v>
       </c>
@@ -63279,7 +63387,7 @@
         <v>236430</v>
       </c>
     </row>
-    <row r="2018" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2018" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2018" s="5" t="s">
         <v>4039</v>
       </c>
@@ -63302,7 +63410,7 @@
         <v>246100</v>
       </c>
     </row>
-    <row r="2019" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2019" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2019" s="3" t="s">
         <v>4041</v>
       </c>
@@ -63325,7 +63433,7 @@
         <v>264370</v>
       </c>
     </row>
-    <row r="2020" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2020" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2020" s="5" t="s">
         <v>4043</v>
       </c>
@@ -63348,7 +63456,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="2021" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2021" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2021" s="3" t="s">
         <v>4045</v>
       </c>
@@ -63371,7 +63479,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="2022" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2022" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2022" s="5" t="s">
         <v>4047</v>
       </c>
@@ -63394,7 +63502,7 @@
         <v>226760</v>
       </c>
     </row>
-    <row r="2023" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="2023" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2023" s="3" t="s">
         <v>4049</v>
       </c>
@@ -63417,7 +63525,7 @@
         <v>373990</v>
       </c>
     </row>
-    <row r="2024" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2024" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2024" s="5" t="s">
         <v>4051</v>
       </c>
@@ -63440,7 +63548,7 @@
         <v>299830</v>
       </c>
     </row>
-    <row r="2025" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2025" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2025" s="3" t="s">
         <v>4053</v>
       </c>
@@ -63463,7 +63571,7 @@
         <v>290160</v>
       </c>
     </row>
-    <row r="2026" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2026" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2026" s="5" t="s">
         <v>4055</v>
       </c>
@@ -63486,7 +63594,7 @@
         <v>241800</v>
       </c>
     </row>
-    <row r="2027" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2027" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2027" s="3" t="s">
         <v>4057</v>
       </c>
@@ -63509,7 +63617,7 @@
         <v>187790</v>
       </c>
     </row>
-    <row r="2028" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2028" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2028" s="5" t="s">
         <v>4059</v>
       </c>
@@ -63532,7 +63640,7 @@
         <v>144010</v>
       </c>
     </row>
-    <row r="2029" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2029" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2029" s="3" t="s">
         <v>4061</v>
       </c>
@@ -63555,7 +63663,7 @@
         <v>270820</v>
       </c>
     </row>
-    <row r="2030" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2030" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2030" s="5" t="s">
         <v>4063</v>
       </c>
@@ -63577,8 +63685,11 @@
       <c r="G2030" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2031" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2030" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2031" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2031" s="3" t="s">
         <v>4065</v>
       </c>
@@ -63601,7 +63712,7 @@
         <v>386880</v>
       </c>
     </row>
-    <row r="2032" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2032" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2032" s="5" t="s">
         <v>4067</v>
       </c>
@@ -63841,8 +63952,8 @@
       <c r="C2042" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2042" s="8" t="s">
-        <v>42</v>
+      <c r="D2042" s="8">
+        <v>1500</v>
       </c>
       <c r="E2042" s="8" t="s">
         <v>42</v>
@@ -64025,8 +64136,8 @@
       <c r="C2050" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2050" s="8" t="s">
-        <v>42</v>
+      <c r="D2050" s="8">
+        <v>1400</v>
       </c>
       <c r="E2050" s="8" t="s">
         <v>42</v>
@@ -64360,7 +64471,7 @@
         <v>174100</v>
       </c>
     </row>
-    <row r="2065" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2065" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2065" s="3" t="s">
         <v>4133</v>
       </c>
@@ -64380,8 +64491,11 @@
       <c r="G2065" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2066" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2065" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2066" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2066" s="5" t="s">
         <v>4135</v>
       </c>
@@ -64404,7 +64518,7 @@
         <v>124660</v>
       </c>
     </row>
-    <row r="2067" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2067" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2067" s="3" t="s">
         <v>4137</v>
       </c>
@@ -64427,7 +64541,7 @@
         <v>329920</v>
       </c>
     </row>
-    <row r="2068" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2068" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2068" s="5" t="s">
         <v>4139</v>
       </c>
@@ -64450,7 +64564,7 @@
         <v>298760</v>
       </c>
     </row>
-    <row r="2069" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2069" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2069" s="3" t="s">
         <v>4141</v>
       </c>
@@ -64473,7 +64587,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="2070" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2070" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2070" s="5" t="s">
         <v>4143</v>
       </c>
@@ -64496,7 +64610,7 @@
         <v>300910</v>
       </c>
     </row>
-    <row r="2071" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2071" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2071" s="3" t="s">
         <v>4145</v>
       </c>
@@ -64519,7 +64633,7 @@
         <v>232130</v>
       </c>
     </row>
-    <row r="2072" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2072" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2072" s="5" t="s">
         <v>4147</v>
       </c>
@@ -64542,7 +64656,7 @@
         <v>370760</v>
       </c>
     </row>
-    <row r="2073" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2073" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2073" s="3" t="s">
         <v>4149</v>
       </c>
@@ -64565,7 +64679,7 @@
         <v>338520</v>
       </c>
     </row>
-    <row r="2074" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2074" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2074" s="5" t="s">
         <v>4151</v>
       </c>
@@ -64588,7 +64702,7 @@
         <v>376130</v>
       </c>
     </row>
-    <row r="2075" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2075" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2075" s="3" t="s">
         <v>4153</v>
       </c>
@@ -64611,7 +64725,7 @@
         <v>299830</v>
       </c>
     </row>
-    <row r="2076" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2076" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2076" s="5" t="s">
         <v>4155</v>
       </c>
@@ -64633,8 +64747,11 @@
       <c r="G2076" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2077" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2076" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2077" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2077" s="3" t="s">
         <v>4157</v>
       </c>
@@ -64656,8 +64773,11 @@
       <c r="G2077" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2078" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2077" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2078" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A2078" s="5" t="s">
         <v>4159</v>
       </c>
@@ -64679,8 +64799,11 @@
       <c r="G2078" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2079" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2078" s="11" t="s">
+        <v>5375</v>
+      </c>
+    </row>
+    <row r="2079" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2079" s="3" t="s">
         <v>4161</v>
       </c>
@@ -64702,8 +64825,11 @@
       <c r="G2079" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2080" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2079" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2080" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2080" s="5" t="s">
         <v>4163</v>
       </c>
@@ -64726,7 +64852,7 @@
         <v>320250</v>
       </c>
     </row>
-    <row r="2081" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2081" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2081" s="3" t="s">
         <v>4165</v>
       </c>
@@ -64749,7 +64875,7 @@
         <v>354640</v>
       </c>
     </row>
-    <row r="2082" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2082" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2082" s="5" t="s">
         <v>4167</v>
       </c>
@@ -64772,7 +64898,7 @@
         <v>346040</v>
       </c>
     </row>
-    <row r="2083" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2083" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2083" s="3" t="s">
         <v>4169</v>
       </c>
@@ -64795,7 +64921,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="2084" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2084" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2084" s="5" t="s">
         <v>4171</v>
       </c>
@@ -64818,7 +64944,7 @@
         <v>186990</v>
       </c>
     </row>
-    <row r="2085" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2085" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2085" s="3" t="s">
         <v>4173</v>
       </c>
@@ -64841,7 +64967,7 @@
         <v>317030</v>
       </c>
     </row>
-    <row r="2086" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2086" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2086" s="5" t="s">
         <v>4175</v>
       </c>
@@ -64864,7 +64990,7 @@
         <v>424490</v>
       </c>
     </row>
-    <row r="2087" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2087" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2087" s="3" t="s">
         <v>4177</v>
       </c>
@@ -64887,7 +65013,7 @@
         <v>327770</v>
       </c>
     </row>
-    <row r="2088" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2088" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2088" s="5" t="s">
         <v>4179</v>
       </c>
@@ -64910,7 +65036,7 @@
         <v>300910</v>
       </c>
     </row>
-    <row r="2089" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2089" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2089" s="3" t="s">
         <v>4181</v>
       </c>
@@ -64930,8 +65056,11 @@
       <c r="G2089" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2090" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2089" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2090" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2090" s="5" t="s">
         <v>4183</v>
       </c>
@@ -64954,7 +65083,7 @@
         <v>118210</v>
       </c>
     </row>
-    <row r="2091" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2091" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2091" s="3" t="s">
         <v>4185</v>
       </c>
@@ -64977,7 +65106,7 @@
         <v>537340</v>
       </c>
     </row>
-    <row r="2092" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2092" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2092" s="5" t="s">
         <v>4187</v>
       </c>
@@ -65000,7 +65129,7 @@
         <v>537340</v>
       </c>
     </row>
-    <row r="2093" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2093" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2093" s="3" t="s">
         <v>4189</v>
       </c>
@@ -65023,7 +65152,7 @@
         <v>537340</v>
       </c>
     </row>
-    <row r="2094" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2094" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2094" s="5" t="s">
         <v>4191</v>
       </c>
@@ -65033,20 +65162,23 @@
       <c r="C2094" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2094" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2094" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2094" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2094" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2095" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2094" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2094" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2094" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2094" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2094" t="s">
+        <v>5376</v>
+      </c>
+    </row>
+    <row r="2095" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2095" s="3" t="s">
         <v>4193</v>
       </c>
@@ -65069,7 +65201,7 @@
         <v>537340</v>
       </c>
     </row>
-    <row r="2096" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="2096" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2096" s="5" t="s">
         <v>4195</v>
       </c>
@@ -65092,7 +65224,7 @@
         <v>352490</v>
       </c>
     </row>
-    <row r="2097" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2097" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2097" s="3" t="s">
         <v>4197</v>
       </c>
@@ -65115,7 +65247,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="2098" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2098" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2098" s="5" t="s">
         <v>4199</v>
       </c>
@@ -65138,7 +65270,7 @@
         <v>494350</v>
       </c>
     </row>
-    <row r="2099" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2099" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2099" s="3" t="s">
         <v>4201</v>
       </c>
@@ -65161,7 +65293,7 @@
         <v>397630</v>
       </c>
     </row>
-    <row r="2100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2100" s="5" t="s">
         <v>4203</v>
       </c>
@@ -65184,7 +65316,7 @@
         <v>349270</v>
       </c>
     </row>
-    <row r="2101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2101" s="3" t="s">
         <v>4205</v>
       </c>
@@ -65207,7 +65339,7 @@
         <v>483600</v>
       </c>
     </row>
-    <row r="2102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2102" s="5" t="s">
         <v>4207</v>
       </c>
@@ -65230,7 +65362,7 @@
         <v>297680</v>
       </c>
     </row>
-    <row r="2103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2103" s="3" t="s">
         <v>4209</v>
       </c>
@@ -65253,7 +65385,7 @@
         <v>456730</v>
       </c>
     </row>
-    <row r="2104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2104" s="5" t="s">
         <v>4211</v>
       </c>
@@ -65276,7 +65408,7 @@
         <v>537340</v>
       </c>
     </row>
-    <row r="2105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2105" s="3" t="s">
         <v>4213</v>
       </c>
@@ -65299,7 +65431,7 @@
         <v>401930</v>
       </c>
     </row>
-    <row r="2106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2106" s="5" t="s">
         <v>4215</v>
       </c>
@@ -65322,7 +65454,7 @@
         <v>537340</v>
       </c>
     </row>
-    <row r="2107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2107" s="3" t="s">
         <v>4217</v>
       </c>
@@ -65342,8 +65474,11 @@
       <c r="G2107" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2107" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2108" s="5" t="s">
         <v>4219</v>
       </c>
@@ -65366,7 +65501,7 @@
         <v>430940</v>
       </c>
     </row>
-    <row r="2109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2109" s="3" t="s">
         <v>4221</v>
       </c>
@@ -65389,7 +65524,7 @@
         <v>193440</v>
       </c>
     </row>
-    <row r="2110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2110" s="5" t="s">
         <v>4223</v>
       </c>
@@ -65412,7 +65547,7 @@
         <v>340670</v>
       </c>
     </row>
-    <row r="2111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2111" s="3" t="s">
         <v>4225</v>
       </c>
@@ -65435,7 +65570,7 @@
         <v>323480</v>
       </c>
     </row>
-    <row r="2112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2112" s="5" t="s">
         <v>4227</v>
       </c>
@@ -65445,20 +65580,23 @@
       <c r="C2112" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2112" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2112" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2112" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2112" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2112" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2112" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2112" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2112" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2112" t="s">
+        <v>5377</v>
+      </c>
+    </row>
+    <row r="2113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2113" s="3" t="s">
         <v>4229</v>
       </c>
@@ -65481,7 +65619,7 @@
         <v>317030</v>
       </c>
     </row>
-    <row r="2114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2114" s="5" t="s">
         <v>4231</v>
       </c>
@@ -65504,7 +65642,7 @@
         <v>300910</v>
       </c>
     </row>
-    <row r="2115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2115" s="3" t="s">
         <v>4233</v>
       </c>
@@ -65527,7 +65665,7 @@
         <v>171950</v>
       </c>
     </row>
-    <row r="2116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2116" s="5" t="s">
         <v>4235</v>
       </c>
@@ -65550,7 +65688,7 @@
         <v>311650</v>
       </c>
     </row>
-    <row r="2117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2117" s="3" t="s">
         <v>4237</v>
       </c>
@@ -65573,7 +65711,7 @@
         <v>296610</v>
       </c>
     </row>
-    <row r="2118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2118" s="5" t="s">
         <v>4239</v>
       </c>
@@ -65596,7 +65734,7 @@
         <v>306280</v>
       </c>
     </row>
-    <row r="2119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2119" s="3" t="s">
         <v>4241</v>
       </c>
@@ -65619,7 +65757,7 @@
         <v>124660</v>
       </c>
     </row>
-    <row r="2120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2120" s="5" t="s">
         <v>4243</v>
       </c>
@@ -65639,8 +65777,11 @@
       <c r="G2120" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2120" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2121" s="3" t="s">
         <v>4245</v>
       </c>
@@ -65663,7 +65804,7 @@
         <v>381510</v>
       </c>
     </row>
-    <row r="2122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2122" s="5" t="s">
         <v>4247</v>
       </c>
@@ -65686,7 +65827,7 @@
         <v>401930</v>
       </c>
     </row>
-    <row r="2123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2123" s="3" t="s">
         <v>4249</v>
       </c>
@@ -65709,7 +65850,7 @@
         <v>300910</v>
       </c>
     </row>
-    <row r="2124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2124" s="5" t="s">
         <v>4251</v>
       </c>
@@ -65732,7 +65873,7 @@
         <v>182690</v>
       </c>
     </row>
-    <row r="2125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2125" s="3" t="s">
         <v>4253</v>
       </c>
@@ -65755,7 +65896,7 @@
         <v>391180</v>
       </c>
     </row>
-    <row r="2126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2126" s="5" t="s">
         <v>4255</v>
       </c>
@@ -65778,7 +65919,7 @@
         <v>318100</v>
       </c>
     </row>
-    <row r="2127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2127" s="3" t="s">
         <v>4257</v>
       </c>
@@ -65788,20 +65929,23 @@
       <c r="C2127" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2127" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2127" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2127" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2127" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2127" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2127" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2127" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2127" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2127" t="s">
+        <v>5378</v>
+      </c>
+    </row>
+    <row r="2128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2128" s="5" t="s">
         <v>4259</v>
       </c>
@@ -66188,7 +66332,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="2145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2145" s="3" t="s">
         <v>4293</v>
       </c>
@@ -66209,7 +66353,7 @@
         <v>186990</v>
       </c>
     </row>
-    <row r="2146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2146" s="5" t="s">
         <v>4295</v>
       </c>
@@ -66232,7 +66376,7 @@
         <v>370760</v>
       </c>
     </row>
-    <row r="2147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2147" s="3" t="s">
         <v>4297</v>
       </c>
@@ -66255,7 +66399,7 @@
         <v>118210</v>
       </c>
     </row>
-    <row r="2148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2148" s="5" t="s">
         <v>4299</v>
       </c>
@@ -66278,7 +66422,7 @@
         <v>306280</v>
       </c>
     </row>
-    <row r="2149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2149" s="3" t="s">
         <v>4301</v>
       </c>
@@ -66301,7 +66445,7 @@
         <v>264370</v>
       </c>
     </row>
-    <row r="2150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2150" s="5" t="s">
         <v>4303</v>
       </c>
@@ -66324,7 +66468,7 @@
         <v>382580</v>
       </c>
     </row>
-    <row r="2151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2151" s="3" t="s">
         <v>4305</v>
       </c>
@@ -66344,8 +66488,11 @@
       <c r="G2151" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2151" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2152" s="5" t="s">
         <v>4307</v>
       </c>
@@ -66368,7 +66515,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="2153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2153" s="3" t="s">
         <v>4309</v>
       </c>
@@ -66391,7 +66538,7 @@
         <v>386880</v>
       </c>
     </row>
-    <row r="2154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2154" s="5" t="s">
         <v>4311</v>
       </c>
@@ -66414,7 +66561,7 @@
         <v>212780</v>
       </c>
     </row>
-    <row r="2155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2155" s="3" t="s">
         <v>4313</v>
       </c>
@@ -66437,7 +66584,7 @@
         <v>408370</v>
       </c>
     </row>
-    <row r="2156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2156" s="5" t="s">
         <v>4315</v>
       </c>
@@ -66460,7 +66607,7 @@
         <v>452440</v>
       </c>
     </row>
-    <row r="2157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2157" s="3" t="s">
         <v>4317</v>
       </c>
@@ -66483,7 +66630,7 @@
         <v>257920</v>
       </c>
     </row>
-    <row r="2158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2158" s="5" t="s">
         <v>4319</v>
       </c>
@@ -66506,7 +66653,7 @@
         <v>365390</v>
       </c>
     </row>
-    <row r="2159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2159" s="3" t="s">
         <v>4321</v>
       </c>
@@ -66529,7 +66676,7 @@
         <v>150450</v>
       </c>
     </row>
-    <row r="2160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2160" s="5" t="s">
         <v>4323</v>
       </c>
@@ -66549,6 +66696,9 @@
       <c r="G2160" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="H2160" s="11" t="s">
+        <v>5342</v>
+      </c>
     </row>
     <row r="2161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2161" s="3" t="s">
@@ -67284,7 +67434,7 @@
         <v>107470</v>
       </c>
     </row>
-    <row r="2193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2193" s="3" t="s">
         <v>4389</v>
       </c>
@@ -67307,7 +67457,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2194" s="5" t="s">
         <v>4391</v>
       </c>
@@ -67330,7 +67480,7 @@
         <v>107470</v>
       </c>
     </row>
-    <row r="2195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2195" s="3" t="s">
         <v>4393</v>
       </c>
@@ -67353,7 +67503,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2196" s="5" t="s">
         <v>4395</v>
       </c>
@@ -67376,7 +67526,7 @@
         <v>128960</v>
       </c>
     </row>
-    <row r="2197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2197" s="3" t="s">
         <v>4397</v>
       </c>
@@ -67399,7 +67549,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2198" s="5" t="s">
         <v>4399</v>
       </c>
@@ -67422,7 +67572,7 @@
         <v>379360</v>
       </c>
     </row>
-    <row r="2199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2199" s="3" t="s">
         <v>4401</v>
       </c>
@@ -67445,7 +67595,7 @@
         <v>225680</v>
       </c>
     </row>
-    <row r="2200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2200" s="5" t="s">
         <v>4403</v>
       </c>
@@ -67468,7 +67618,7 @@
         <v>247170</v>
       </c>
     </row>
-    <row r="2201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2201" s="3" t="s">
         <v>4405</v>
       </c>
@@ -67491,7 +67641,7 @@
         <v>224610</v>
       </c>
     </row>
-    <row r="2202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2202" s="5" t="s">
         <v>4407</v>
       </c>
@@ -67514,7 +67664,7 @@
         <v>265440</v>
       </c>
     </row>
-    <row r="2203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2203" s="3" t="s">
         <v>4409</v>
       </c>
@@ -67537,7 +67687,7 @@
         <v>331000</v>
       </c>
     </row>
-    <row r="2204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2204" s="5" t="s">
         <v>4411</v>
       </c>
@@ -67560,7 +67710,7 @@
         <v>285860</v>
       </c>
     </row>
-    <row r="2205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2205" s="3" t="s">
         <v>4413</v>
       </c>
@@ -67570,8 +67720,8 @@
       <c r="C2205" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2205" s="7" t="s">
-        <v>42</v>
+      <c r="D2205" s="7">
+        <v>950</v>
       </c>
       <c r="E2205" s="7" t="s">
         <v>42</v>
@@ -67583,7 +67733,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2206" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="2206" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2206" s="5" t="s">
         <v>4415</v>
       </c>
@@ -67603,8 +67753,11 @@
       <c r="G2206" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2207" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="H2206" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2207" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2207" s="3" t="s">
         <v>4417</v>
       </c>
@@ -67626,8 +67779,11 @@
       <c r="G2207" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2207" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2208" s="5" t="s">
         <v>4419</v>
       </c>
@@ -67650,7 +67806,7 @@
         <v>375060</v>
       </c>
     </row>
-    <row r="2209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2209" s="3" t="s">
         <v>4421</v>
       </c>
@@ -67673,7 +67829,7 @@
         <v>375060</v>
       </c>
     </row>
-    <row r="2210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2210" s="5" t="s">
         <v>4423</v>
       </c>
@@ -67693,8 +67849,11 @@
       <c r="G2210" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2210" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2211" s="3" t="s">
         <v>4425</v>
       </c>
@@ -67714,8 +67873,11 @@
       <c r="G2211" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2211" s="10" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2212" s="5" t="s">
         <v>4427</v>
       </c>
@@ -67735,8 +67897,11 @@
       <c r="G2212" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2212" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2213" s="3" t="s">
         <v>4429</v>
       </c>
@@ -67757,7 +67922,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="2214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2214" s="5" t="s">
         <v>4431</v>
       </c>
@@ -67777,8 +67942,11 @@
       <c r="G2214" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2215" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2214" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2215" s="3" t="s">
         <v>4433</v>
       </c>
@@ -67788,20 +67956,23 @@
       <c r="C2215" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2215" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2215" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2215" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2215" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2216" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2215" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2215" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2215" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2215" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2215" t="s">
+        <v>5323</v>
+      </c>
+    </row>
+    <row r="2216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2216" s="5" t="s">
         <v>4435</v>
       </c>
@@ -67811,20 +67982,23 @@
       <c r="C2216" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2216" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2216" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2216" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2216" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2217" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2216" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2216" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2216" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2216" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2216" t="s">
+        <v>5323</v>
+      </c>
+    </row>
+    <row r="2217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2217" s="3" t="s">
         <v>4437</v>
       </c>
@@ -67847,7 +68021,7 @@
         <v>209560</v>
       </c>
     </row>
-    <row r="2218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2218" s="5" t="s">
         <v>4439</v>
       </c>
@@ -67867,8 +68041,11 @@
       <c r="G2218" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2219" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2218" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2219" s="3" t="s">
         <v>4441</v>
       </c>
@@ -67888,8 +68065,11 @@
       <c r="G2219" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2220" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2219" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2220" s="5" t="s">
         <v>4443</v>
       </c>
@@ -67912,7 +68092,7 @@
         <v>214930</v>
       </c>
     </row>
-    <row r="2221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2221" s="3" t="s">
         <v>4445</v>
       </c>
@@ -67932,8 +68112,11 @@
       <c r="G2221" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2222" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2221" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2222" s="5" t="s">
         <v>4447</v>
       </c>
@@ -67953,8 +68136,11 @@
       <c r="G2222" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2223" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2222" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2223" s="3" t="s">
         <v>4449</v>
       </c>
@@ -67974,8 +68160,11 @@
       <c r="G2223" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2224" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2223" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2224" s="5" t="s">
         <v>4451</v>
       </c>
@@ -67995,8 +68184,11 @@
       <c r="G2224" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2225" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="H2224" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2225" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2225" s="3" t="s">
         <v>4453</v>
       </c>
@@ -68016,8 +68208,11 @@
       <c r="G2225" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2226" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2225" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2226" s="5" t="s">
         <v>4455</v>
       </c>
@@ -68040,7 +68235,7 @@
         <v>153680</v>
       </c>
     </row>
-    <row r="2227" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2227" s="3" t="s">
         <v>4457</v>
       </c>
@@ -68060,8 +68255,11 @@
       <c r="G2227" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2228" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2227" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2228" s="5" t="s">
         <v>4459</v>
       </c>
@@ -68082,7 +68280,7 @@
         <v>252550</v>
       </c>
     </row>
-    <row r="2229" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2229" s="3" t="s">
         <v>4461</v>
       </c>
@@ -68105,7 +68303,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="2230" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="2230" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2230" s="5" t="s">
         <v>4463</v>
       </c>
@@ -68125,8 +68323,11 @@
       <c r="G2230" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2230" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2231" s="3" t="s">
         <v>4465</v>
       </c>
@@ -68149,7 +68350,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="2232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2232" s="5" t="s">
         <v>4467</v>
       </c>
@@ -68170,7 +68371,7 @@
         <v>322400</v>
       </c>
     </row>
-    <row r="2233" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="2233" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2233" s="3" t="s">
         <v>4469</v>
       </c>
@@ -68190,8 +68391,11 @@
       <c r="G2233" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2234" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2233" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2234" s="5" t="s">
         <v>4471</v>
       </c>
@@ -68211,8 +68415,11 @@
       <c r="G2234" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2235" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2234" s="11" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2235" s="3" t="s">
         <v>4473</v>
       </c>
@@ -68235,7 +68442,7 @@
         <v>204190</v>
       </c>
     </row>
-    <row r="2236" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2236" s="5" t="s">
         <v>4475</v>
       </c>
@@ -68258,7 +68465,7 @@
         <v>268670</v>
       </c>
     </row>
-    <row r="2237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2237" s="3" t="s">
         <v>4477</v>
       </c>
@@ -68268,20 +68475,23 @@
       <c r="C2237" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2237" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2237" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2237" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2237" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2238" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2237" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2237" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2237" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2237" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2237" t="s">
+        <v>5323</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2238" s="5" t="s">
         <v>4479</v>
       </c>
@@ -68291,20 +68501,23 @@
       <c r="C2238" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2238" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2238" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2238" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2238" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2239" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2238" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2238" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2238" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2238" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2238" t="s">
+        <v>5379</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2239" s="3" t="s">
         <v>4481</v>
       </c>
@@ -68314,20 +68527,23 @@
       <c r="C2239" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2239" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2239" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2239" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2239" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2240" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2239" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2239" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2239" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2239" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2239" t="s">
+        <v>5379</v>
+      </c>
+    </row>
+    <row r="2240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2240" s="5" t="s">
         <v>4483</v>
       </c>
@@ -68416,6 +68632,9 @@
       <c r="G2243" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="H2243" s="10" t="s">
+        <v>5342</v>
+      </c>
     </row>
     <row r="2244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2244" s="5" t="s">
@@ -68437,6 +68656,9 @@
       <c r="G2244" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="H2244" s="11" t="s">
+        <v>5342</v>
+      </c>
     </row>
     <row r="2245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2245" s="3" t="s">
@@ -68481,6 +68703,9 @@
       <c r="G2246" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="H2246" s="11" t="s">
+        <v>5342</v>
+      </c>
     </row>
     <row r="2247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2247" s="3" t="s">
@@ -68548,6 +68773,9 @@
       <c r="G2249" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="H2249" s="10" t="s">
+        <v>5342</v>
+      </c>
     </row>
     <row r="2250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2250" s="5" t="s">
@@ -68569,6 +68797,9 @@
       <c r="G2250" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="H2250" s="11" t="s">
+        <v>5342</v>
+      </c>
     </row>
     <row r="2251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2251" s="3" t="s">
@@ -68613,6 +68844,9 @@
       <c r="G2252" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="H2252" s="11" t="s">
+        <v>5342</v>
+      </c>
     </row>
     <row r="2253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2253" s="3" t="s">
@@ -77696,131 +77930,131 @@
     </row>
     <row r="2647" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2648" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2648" s="14" t="s">
+      <c r="A2648" s="13" t="s">
         <v>5297</v>
       </c>
-      <c r="B2648" s="14"/>
-      <c r="C2648" s="14"/>
-      <c r="D2648" s="14"/>
-      <c r="E2648" s="14"/>
-      <c r="F2648" s="14"/>
-      <c r="G2648" s="14"/>
+      <c r="B2648" s="13"/>
+      <c r="C2648" s="13"/>
+      <c r="D2648" s="13"/>
+      <c r="E2648" s="13"/>
+      <c r="F2648" s="13"/>
+      <c r="G2648" s="13"/>
     </row>
     <row r="2649" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2649" s="1" t="s">
         <v>5298</v>
       </c>
-      <c r="B2649" s="14" t="s">
+      <c r="B2649" s="13" t="s">
         <v>5299</v>
       </c>
-      <c r="C2649" s="14"/>
-      <c r="D2649" s="14"/>
-      <c r="E2649" s="14"/>
-      <c r="F2649" s="14"/>
-      <c r="G2649" s="14"/>
+      <c r="C2649" s="13"/>
+      <c r="D2649" s="13"/>
+      <c r="E2649" s="13"/>
+      <c r="F2649" s="13"/>
+      <c r="G2649" s="13"/>
     </row>
     <row r="2650" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2650" s="14" t="s">
+      <c r="B2650" s="13" t="s">
         <v>5300</v>
       </c>
-      <c r="C2650" s="14"/>
-      <c r="D2650" s="14"/>
-      <c r="E2650" s="14"/>
-      <c r="F2650" s="14"/>
-      <c r="G2650" s="14"/>
+      <c r="C2650" s="13"/>
+      <c r="D2650" s="13"/>
+      <c r="E2650" s="13"/>
+      <c r="F2650" s="13"/>
+      <c r="G2650" s="13"/>
     </row>
     <row r="2651" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2651" s="14" t="s">
+      <c r="B2651" s="13" t="s">
         <v>5301</v>
       </c>
-      <c r="C2651" s="14"/>
-      <c r="D2651" s="14"/>
-      <c r="E2651" s="14"/>
-      <c r="F2651" s="14"/>
-      <c r="G2651" s="14"/>
+      <c r="C2651" s="13"/>
+      <c r="D2651" s="13"/>
+      <c r="E2651" s="13"/>
+      <c r="F2651" s="13"/>
+      <c r="G2651" s="13"/>
     </row>
     <row r="2652" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2652" s="14" t="s">
+      <c r="B2652" s="13" t="s">
         <v>5302</v>
       </c>
-      <c r="C2652" s="14"/>
-      <c r="D2652" s="14"/>
-      <c r="E2652" s="14"/>
-      <c r="F2652" s="14"/>
-      <c r="G2652" s="14"/>
+      <c r="C2652" s="13"/>
+      <c r="D2652" s="13"/>
+      <c r="E2652" s="13"/>
+      <c r="F2652" s="13"/>
+      <c r="G2652" s="13"/>
     </row>
     <row r="2653" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2653" s="14" t="s">
+      <c r="B2653" s="13" t="s">
         <v>5303</v>
       </c>
-      <c r="C2653" s="14"/>
-      <c r="D2653" s="14"/>
-      <c r="E2653" s="14"/>
-      <c r="F2653" s="14"/>
-      <c r="G2653" s="14"/>
+      <c r="C2653" s="13"/>
+      <c r="D2653" s="13"/>
+      <c r="E2653" s="13"/>
+      <c r="F2653" s="13"/>
+      <c r="G2653" s="13"/>
     </row>
     <row r="2654" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2654" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B2654" s="14" t="s">
+      <c r="B2654" s="13" t="s">
         <v>5304</v>
       </c>
-      <c r="C2654" s="14"/>
-      <c r="D2654" s="14"/>
-      <c r="E2654" s="14"/>
-      <c r="F2654" s="14"/>
-      <c r="G2654" s="14"/>
+      <c r="C2654" s="13"/>
+      <c r="D2654" s="13"/>
+      <c r="E2654" s="13"/>
+      <c r="F2654" s="13"/>
+      <c r="G2654" s="13"/>
     </row>
     <row r="2655" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2655" s="14" t="s">
+      <c r="B2655" s="13" t="s">
         <v>5305</v>
       </c>
-      <c r="C2655" s="14"/>
-      <c r="D2655" s="14"/>
-      <c r="E2655" s="14"/>
-      <c r="F2655" s="14"/>
-      <c r="G2655" s="14"/>
+      <c r="C2655" s="13"/>
+      <c r="D2655" s="13"/>
+      <c r="E2655" s="13"/>
+      <c r="F2655" s="13"/>
+      <c r="G2655" s="13"/>
     </row>
     <row r="2656" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2656" s="14" t="s">
+      <c r="B2656" s="13" t="s">
         <v>5306</v>
       </c>
-      <c r="C2656" s="14"/>
-      <c r="D2656" s="14"/>
-      <c r="E2656" s="14"/>
-      <c r="F2656" s="14"/>
-      <c r="G2656" s="14"/>
+      <c r="C2656" s="13"/>
+      <c r="D2656" s="13"/>
+      <c r="E2656" s="13"/>
+      <c r="F2656" s="13"/>
+      <c r="G2656" s="13"/>
     </row>
     <row r="2657" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2657" s="14" t="s">
+      <c r="B2657" s="13" t="s">
         <v>5307</v>
       </c>
-      <c r="C2657" s="14"/>
-      <c r="D2657" s="14"/>
-      <c r="E2657" s="14"/>
-      <c r="F2657" s="14"/>
-      <c r="G2657" s="14"/>
+      <c r="C2657" s="13"/>
+      <c r="D2657" s="13"/>
+      <c r="E2657" s="13"/>
+      <c r="F2657" s="13"/>
+      <c r="G2657" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:G2646" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="16">
-    <mergeCell ref="B2653:G2653"/>
-    <mergeCell ref="B2654:G2654"/>
-    <mergeCell ref="B2655:G2655"/>
-    <mergeCell ref="B2656:G2656"/>
-    <mergeCell ref="B2657:G2657"/>
-    <mergeCell ref="A2648:G2648"/>
-    <mergeCell ref="B2649:G2649"/>
-    <mergeCell ref="B2650:G2650"/>
-    <mergeCell ref="B2651:G2651"/>
-    <mergeCell ref="B2652:G2652"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A2648:G2648"/>
+    <mergeCell ref="B2649:G2649"/>
+    <mergeCell ref="B2650:G2650"/>
+    <mergeCell ref="B2651:G2651"/>
+    <mergeCell ref="B2652:G2652"/>
+    <mergeCell ref="B2653:G2653"/>
+    <mergeCell ref="B2654:G2654"/>
+    <mergeCell ref="B2655:G2655"/>
+    <mergeCell ref="B2656:G2656"/>
+    <mergeCell ref="B2657:G2657"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>